<commit_message>
1) add more data cleaning 2) fix Borda scores 20 -> 12 3) generate topster diagrams
</commit_message>
<xml_diff>
--- a/output/TopReleasesByNum1Votes.xlsx
+++ b/output/TopReleasesByNum1Votes.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t xml:space="preserve">Artist</t>
   </si>
@@ -24,108 +24,6 @@
   </si>
   <si>
     <t xml:space="preserve">TitletoLowercase</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J.P.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bad Bitty</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bad bitty</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adrianne Lenker</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bright Future</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bright future</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bladee</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cold Visions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cold visions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MJ Nebreda, Danny From Miami, Danny Daze</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Con Cariño</t>
-  </si>
-  <si>
-    <t xml:space="preserve">con cariño</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gawshock</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cool Drink</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cool drink</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DJ Sabrina The Teenage DJ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hex</t>
-  </si>
-  <si>
-    <t xml:space="preserve">hex</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JPEGMAFIA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I LAY DOWN MY LIFE FOR YOU</t>
-  </si>
-  <si>
-    <t xml:space="preserve">i lay down my life for you</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Otomekaiga</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kyoukai</t>
-  </si>
-  <si>
-    <t xml:space="preserve">kyoukai</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Parannoul</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sky Hundred</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sky hundred</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fontaines D.C.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Starburster</t>
-  </si>
-  <si>
-    <t xml:space="preserve">starburster</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Marías</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Submarine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">submarine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Maria's</t>
   </si>
 </sst>
 </file>
@@ -471,174 +369,6 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="n">
-        <v>20</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="n">
-        <v>20</v>
-      </c>
-      <c r="D3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="n">
-        <v>20</v>
-      </c>
-      <c r="D4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" t="n">
-        <v>20</v>
-      </c>
-      <c r="D5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" t="n">
-        <v>20</v>
-      </c>
-      <c r="D6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B7" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" t="n">
-        <v>20</v>
-      </c>
-      <c r="D7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" t="n">
-        <v>20</v>
-      </c>
-      <c r="D8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" t="s">
-        <v>26</v>
-      </c>
-      <c r="C9" t="n">
-        <v>20</v>
-      </c>
-      <c r="D9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10" t="s">
-        <v>29</v>
-      </c>
-      <c r="C10" t="n">
-        <v>20</v>
-      </c>
-      <c r="D10" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="s">
-        <v>31</v>
-      </c>
-      <c r="B11" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11" t="n">
-        <v>20</v>
-      </c>
-      <c r="D11" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="s">
-        <v>34</v>
-      </c>
-      <c r="B12" t="s">
-        <v>35</v>
-      </c>
-      <c r="C12" t="n">
-        <v>20</v>
-      </c>
-      <c r="D12" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="s">
-        <v>37</v>
-      </c>
-      <c r="B13" t="s">
-        <v>35</v>
-      </c>
-      <c r="C13" t="n">
-        <v>20</v>
-      </c>
-      <c r="D13" t="s">
-        <v>36</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>

</xml_diff>